<commit_message>
added CMakeList, deleted Rump–Ogita–Oishi algorithm
</commit_message>
<xml_diff>
--- a/Reports.xlsx
+++ b/Reports.xlsx
@@ -19,24 +19,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>float</t>
   </si>
   <si>
     <t>double</t>
-  </si>
-  <si>
-    <t>1 случай</t>
-  </si>
-  <si>
-    <t>2 случай</t>
-  </si>
-  <si>
-    <t>Cуммирование без алгоритма Rump–Ogita–Oishi</t>
-  </si>
-  <si>
-    <t>Cуммирование через алгоритм Rump–Ogita–Oishi</t>
   </si>
   <si>
     <t>строки - типы данных</t>
@@ -101,12 +89,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -125,487 +116,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="ru-RU"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="ru-RU"/>
-              <a:t>Производительность, 1</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>e6 </a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="ru-RU"/>
-              <a:t>отсчетов/сек</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$4</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>float</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$3:$H$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>128</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$4:$H$4</c:f>
-              <c:numCache>
-                <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>2.8985509999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>2.808989</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.9850750000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.030303</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.0487799999999998</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.039514</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-7CF9-4D7D-8139-B25F94FEFF8D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$B$5</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>double</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:cat>
-            <c:numRef>
-              <c:f>Sheet1!$C$3:$H$3</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>8</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>16</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>32</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>64</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>128</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$5:$H$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.00000</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>3.4129689999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.2573289999999999</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.5842290000000001</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.5842290000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.5842290000000001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.5971220000000002</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7CF9-4D7D-8139-B25F94FEFF8D}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="602974239"/>
-        <c:axId val="602976319"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="602974239"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="602976319"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="602976319"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="4.3"/>
-          <c:min val="2.7"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="0.00000" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="ru-RU"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="602974239"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="b"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="ru-RU"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="ru-RU"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ru-RU"/>
@@ -1130,46 +640,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
@@ -1673,541 +1143,8 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>7620</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>179070</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>179070</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Диаграмма 3"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
@@ -2232,7 +1169,7 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2507,29 +1444,21 @@
   <dimension ref="B2:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+      <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="J2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>4</v>
-      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="2"/>
       <c r="L2" s="2"/>
       <c r="M2" s="2"/>
       <c r="N2" s="2"/>
@@ -2537,25 +1466,13 @@
       <c r="P2" s="2"/>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B3" s="1"/>
-      <c r="C3" s="1">
-        <v>4</v>
-      </c>
-      <c r="D3" s="1">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1">
-        <v>16</v>
-      </c>
-      <c r="F3" s="1">
-        <v>32</v>
-      </c>
-      <c r="G3" s="1">
-        <v>64</v>
-      </c>
-      <c r="H3" s="1">
-        <v>128</v>
-      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1">
         <v>4</v>
@@ -2576,31 +1493,17 @@
         <v>128</v>
       </c>
       <c r="R3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>2.8985509999999999</v>
-      </c>
-      <c r="D4" s="4">
-        <v>2.808989</v>
-      </c>
-      <c r="E4" s="4">
-        <v>2.9850750000000001</v>
-      </c>
-      <c r="F4" s="4">
-        <v>3.030303</v>
-      </c>
-      <c r="G4" s="4">
-        <v>3.0487799999999998</v>
-      </c>
-      <c r="H4" s="4">
-        <v>3.039514</v>
-      </c>
+      <c r="B4" s="6"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
       <c r="J4" s="1" t="s">
         <v>0</v>
       </c>
@@ -2623,31 +1526,17 @@
         <v>3.558719</v>
       </c>
       <c r="R4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B5" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="4">
-        <v>3.4129689999999999</v>
-      </c>
-      <c r="D5" s="4">
-        <v>3.2573289999999999</v>
-      </c>
-      <c r="E5" s="4">
-        <v>3.5842290000000001</v>
-      </c>
-      <c r="F5" s="4">
-        <v>3.5842290000000001</v>
-      </c>
-      <c r="G5" s="4">
-        <v>3.5842290000000001</v>
-      </c>
-      <c r="H5" s="4">
-        <v>3.5971220000000002</v>
-      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
       <c r="J5" s="1" t="s">
         <v>1</v>
       </c>

</xml_diff>